<commit_message>
rev b to fab
</commit_message>
<xml_diff>
--- a/hardware/power_supply_module/rev_b/power_supply_module_bom.xlsx
+++ b/hardware/power_supply_module/rev_b/power_supply_module_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="power_supply_module" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">DIGIKEY</t>
   </si>
   <si>
+    <t xml:space="preserve">0.017 Ohm</t>
+  </si>
+  <si>
     <t xml:space="preserve">RESISTOR0805_RES</t>
   </si>
   <si>
@@ -58,7 +61,7 @@
     <t xml:space="preserve">WSLPB-.017CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">100k</t>
+    <t xml:space="preserve">10 kOhm</t>
   </si>
   <si>
     <t xml:space="preserve">RESISTOR0402_RES</t>
@@ -67,49 +70,58 @@
     <t xml:space="preserve">0402_RES</t>
   </si>
   <si>
-    <t xml:space="preserve">R9, R10, R11, R12, R13</t>
+    <t xml:space="preserve">R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10KJCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 kOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R33, R34, R35, R36, R37</t>
   </si>
   <si>
     <t xml:space="preserve">P100KJCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">130k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R14, R15, R16, R17</t>
+    <t xml:space="preserve">130 kOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R38, R39, R40, R41</t>
   </si>
   <si>
     <t xml:space="preserve">P130KLCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">240k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R18</t>
+    <t xml:space="preserve">240 kOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R42</t>
   </si>
   <si>
     <t xml:space="preserve">P240KLCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">680k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R19, R20, R21, R22</t>
+    <t xml:space="preserve">680 kOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R43, R44, R45, R46</t>
   </si>
   <si>
     <t xml:space="preserve">P680KLCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">750k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R23</t>
+    <t xml:space="preserve">750 kOhm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R47</t>
   </si>
   <si>
     <t xml:space="preserve">P750KLCT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">3.3n</t>
+    <t xml:space="preserve">3.3 nF</t>
   </si>
   <si>
     <t xml:space="preserve">CAPACITOR0402_CAP</t>
@@ -127,7 +139,7 @@
     <t xml:space="preserve">490-3248-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1u</t>
+    <t xml:space="preserve">0.1 uF</t>
   </si>
   <si>
     <t xml:space="preserve">C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18</t>
@@ -136,27 +148,30 @@
     <t xml:space="preserve">490-5920-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">10u</t>
+    <t xml:space="preserve">10 uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPACITOR0805_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805_CAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C19, C20, C21, C22, C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805 Capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-5523-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 uF</t>
   </si>
   <si>
     <t xml:space="preserve">CAPACITOR0603_CAP</t>
   </si>
   <si>
-    <t xml:space="preserve">0805_CAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C19, C20, C21, C22, C23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0805 Capacitor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-5523-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22u</t>
-  </si>
-  <si>
     <t xml:space="preserve">0603_CAP</t>
   </si>
   <si>
@@ -169,7 +184,7 @@
     <t xml:space="preserve">1276-1193-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">2.2u</t>
+    <t xml:space="preserve">2.2 uH</t>
   </si>
   <si>
     <t xml:space="preserve">INDUCTORIHL</t>
@@ -187,6 +202,63 @@
     <t xml:space="preserve">541-1322-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">LTC2941</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DFN-6-2MMX3MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U8, U9, U10, U11, U12, U13, U14, U15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I2C Battery Gas Gauge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTC2941IDCB#TRMPBFCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODULE_POWER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header for power module for signpost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S9172-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCA9544AQFN-N20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QFN-N20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6, U7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-4 I2C/SMBUS Multiplexer with interrupt for power supply coulomb counters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">296-20960-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST_POINT_0.040IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTPOINT_0.040IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">!INT, 3V3, 5V_1, 5V_2, 5V_3, 5V_4, BACK, GND, LINUX, MOD0, MOD1, MOD2, MOD5, MOD6, MOD7, SCL, SDA, VBATT, VSOL+, VSOL-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.040in Test Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5001K-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">TLV62130</t>
   </si>
   <si>
@@ -200,36 +272,6 @@
   </si>
   <si>
     <t xml:space="preserve">296-35978-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCA9544A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SO20L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U6, U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-4 I2C/SMBUS Multiplexer with interrupt for power supply coulomb counters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">296-20958-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTC2941</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DFN-6-2MMX3MM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U8, U9, U10, U11, U12, U13, U14, U15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I2C Battery Gas Gauge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTC2941IDCB#TRMPBFCT-ND</t>
   </si>
 </sst>
 </file>
@@ -304,8 +346,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -326,10 +372,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -337,8 +383,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.7091836734694"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="62.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="75.7295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.234693877551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3214285714286"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
@@ -370,207 +416,207 @@
       <c r="A2" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>0.017</v>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>11</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>25</v>
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>28</v>
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="F8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>31</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>37</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -578,45 +624,45 @@
         <v>5</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="E12" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>55</v>
@@ -644,7 +690,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>60</v>
@@ -667,7 +713,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>65</v>
@@ -676,16 +722,85 @@
         <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>69</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Listed locations for purchasing parts
</commit_message>
<xml_diff>
--- a/hardware/power_supply_module/rev_b/power_supply_module_bom.xlsx
+++ b/hardware/power_supply_module/rev_b/power_supply_module_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="power_supply_module" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
   <si>
     <t xml:space="preserve">Qty</t>
   </si>
@@ -166,6 +166,9 @@
     <t xml:space="preserve">490-5523-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">Out of stock: Substituting 587-2985-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">22 uF</t>
   </si>
   <si>
@@ -229,6 +232,9 @@
     <t xml:space="preserve">S9172-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">signpost</t>
+  </si>
+  <si>
     <t xml:space="preserve">PCA9544AQFN-N20</t>
   </si>
   <si>
@@ -257,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve">5001K-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stock</t>
   </si>
   <si>
     <t xml:space="preserve">TLV62130</t>
@@ -372,21 +381,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="75.7295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.234693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.7142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.9183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,28 +649,31 @@
       <c r="G11" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="I11" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -670,22 +681,22 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,22 +704,22 @@
         <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,22 +727,25 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,22 +753,22 @@
         <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -762,22 +776,25 @@
         <v>20</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -785,22 +802,22 @@
         <v>5</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use 2kOhm resistors for gauges. Fixes #13
</commit_message>
<xml_diff>
--- a/hardware/power_supply_module/rev_b/power_supply_module_bom.xlsx
+++ b/hardware/power_supply_module/rev_b/power_supply_module_bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="997" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="power_supply_module" sheetId="1" state="visible" r:id="rId2"/>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">R9, R10, R11, R12, R13, R14, R15, R16, R17, R18, R19, R20, R21, R22, R23, R24, R25, R26, R27, R28, R29, R30, R31, R32</t>
   </si>
   <si>
-    <t xml:space="preserve">P10KJCT-ND</t>
+    <t xml:space="preserve">P2.00KLCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">100 kOhm</t>
@@ -384,17 +384,18 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.18367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="118.938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="117.714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>